<commit_message>
EPBDS-6900 Add a test on casting from SR to CustomSR
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/CastOfCustomSpreadsheetResult.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/CastOfCustomSpreadsheetResult.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="27795" windowHeight="12585" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t>Spreadsheet SpreadsheetResult Test1 (Double a)</t>
   </si>
@@ -34,60 +35,9 @@
     <t>Spreadsheet SpreadsheetResult Test2 (Double[] a, Double b)</t>
   </si>
   <si>
-    <t>step2</t>
-  </si>
-  <si>
     <t>= Test1(a)</t>
   </si>
   <si>
-    <t>Spreadsheet SpreadsheetResult Test3 (Double[] a, Double[] b)</t>
-  </si>
-  <si>
-    <t>= Test2(a,b)</t>
-  </si>
-  <si>
-    <t>step3</t>
-  </si>
-  <si>
-    <t>= $value$step2($step2)</t>
-  </si>
-  <si>
-    <t>step4</t>
-  </si>
-  <si>
-    <t>= (SpreadsheetResultTest1[])flatten($step3)</t>
-  </si>
-  <si>
-    <t>step5</t>
-  </si>
-  <si>
-    <t>= (SpreadsheetResult[]) $step4</t>
-  </si>
-  <si>
-    <t>step2 : SpreadsheetResultTest1</t>
-  </si>
-  <si>
-    <t>step2 : SpreadsheetResult[]</t>
-  </si>
-  <si>
-    <t>= (StpreadsheetResult[]) Test1(a)</t>
-  </si>
-  <si>
-    <t>= (SpreadsheetResult[]) Test1(a)</t>
-  </si>
-  <si>
-    <t>step2 : SpreadsheetResultTest1[]</t>
-  </si>
-  <si>
-    <t>step3 : SpreadsheetResult</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t xml:space="preserve">= </t>
-  </si>
-  <si>
     <t>= (SpreadsheetResult[]) $step2</t>
   </si>
   <si>
@@ -112,9 +62,6 @@
     <t>B</t>
   </si>
   <si>
-    <t>_res_</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
@@ -124,21 +71,65 @@
     <t>2</t>
   </si>
   <si>
-    <t>_res_.$value$step3.$value$step1</t>
-  </si>
-  <si>
     <t>_res_.$value$step3[0].$value$step1</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult TWO(String var)</t>
+  </si>
+  <si>
+    <t>Step</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Res</t>
+  </si>
+  <si>
+    <t>=ONE ( null )</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult Total(String val2)</t>
+  </si>
+  <si>
+    <t>Tot:SpreadsheetResultTWO</t>
+  </si>
+  <si>
+    <t>=TWO( null )</t>
+  </si>
+  <si>
+    <t>Res2</t>
+  </si>
+  <si>
+    <t>=$Formula$Res($Tot)</t>
+  </si>
+  <si>
+    <t>Res3</t>
+  </si>
+  <si>
+    <t>=$Formula$ten($Res2)</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult ONE( String str)</t>
+  </si>
+  <si>
+    <t>ten</t>
+  </si>
+  <si>
+    <t>Test Total MyTest</t>
+  </si>
+  <si>
+    <t>_res_.$Formula$Res3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1" rgb="FFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -157,7 +148,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -207,37 +198,37 @@
       <diagonal/>
     </border>
     <border>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,147 +531,241 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:F24"/>
+  <dimension ref="B4:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="54.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="41.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="3" max="3" width="54.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="41" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>0</v>
       </c>
       <c r="D4" s="5"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C5" s="2" t="s">
+    </row>
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C6" s="2" t="s">
+    </row>
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="8" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C9" s="2" t="s">
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D10" s="3" t="s">
+    </row>
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11">
-      <c r="C11" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="3:6" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="3:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="3:5" ht="15.75" x14ac:dyDescent="0.3">
-      <c r="E18" s="1"/>
-    </row>
-    <row r="21" spans="3:5" ht="15.75" x14ac:dyDescent="0.3"/>
-    <row r="22" spans="3:5" ht="15.75" x14ac:dyDescent="0.3"/>
-    <row r="23" spans="3:5" ht="15.75" x14ac:dyDescent="0.3"/>
-    <row r="24" spans="3:5" ht="15.75" x14ac:dyDescent="0.3"/>
-    <row r="26">
-      <c r="B26" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-    </row>
-    <row r="27">
-      <c r="B27" t="s" s="7">
-        <v>28</v>
-      </c>
-      <c r="C27" t="s" s="7">
-        <v>30</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="B28" t="s" s="7">
-        <v>29</v>
-      </c>
-      <c r="C28" t="s" s="7">
-        <v>31</v>
-      </c>
-      <c r="D28" t="s" s="7">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="B29" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>34</v>
+    </row>
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C8:D8"/>
-    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B15:D15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:C26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="26" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="8"/>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="8"/>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="3">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>